<commit_message>
Mexi na planilha de homo
</commit_message>
<xml_diff>
--- a/documentacao/planilha-de-homo/Plano-de-UAT-homologacao.xlsx
+++ b/documentacao/planilha-de-homo/Plano-de-UAT-homologacao.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\BandTec\1º Semestre\Pesquisa e Inovação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Regin\OneDrive\Documents\PI\paiotnela\documentacao\planilha-de-homo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AD05F5-ECB6-4C07-B8FD-B2ED660A6244}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8986EE80-9C64-4772-924D-BBA97AF6FE1F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="596" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="596" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Homologação" sheetId="5" r:id="rId1"/>
-    <sheet name="Cenário 1 - Cadastro" sheetId="7" r:id="rId2"/>
+    <sheet name="Cenário 1 - Cadastro" sheetId="9" r:id="rId2"/>
     <sheet name="Cenário 2 - Login" sheetId="6" r:id="rId3"/>
     <sheet name="." sheetId="4" r:id="rId4"/>
-    <sheet name="Cenário 3 - Dashboard" sheetId="8" r:id="rId5"/>
+    <sheet name="Cenário 3 - Dashboard" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="134">
   <si>
     <t xml:space="preserve">Projeto: </t>
   </si>
@@ -197,15 +197,6 @@
     <t>Logar no sistema</t>
   </si>
   <si>
-    <t>Código do Cliente:</t>
-  </si>
-  <si>
-    <t>Logar no sistema, clicar na opção de busca do cliente no menu principal, digitar o CÓDIGO do cliente.</t>
-  </si>
-  <si>
-    <t>Ao deixar em branco o campo e preencher, o sistema deverá fornecer um aviso que o código está em branco e não deve permitir a busca.</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -281,12 +272,6 @@
     <t xml:space="preserve">Permitir o login no sistema utilizando email e senha	</t>
   </si>
   <si>
-    <t xml:space="preserve">Consistir o campo "Login" com email válido	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consistir o campo "Senha" com dados válidos	</t>
-  </si>
-  <si>
     <t>XXXX</t>
   </si>
   <si>
@@ -422,19 +407,52 @@
     <t>RF002-TC003</t>
   </si>
   <si>
-    <t>RF002-TC004</t>
-  </si>
-  <si>
-    <t>RF002-TC005</t>
-  </si>
-  <si>
-    <t>O sistema deve concluir o login e redirecionar o usuário para a Dash, com a mensagem: "Bem vindo (nome do usuário)!"</t>
-  </si>
-  <si>
     <t>Condição/Interação com sistema</t>
   </si>
   <si>
-    <t>Logar no sistema, clicar na opção de busca do cliente no menu principal, dig</t>
+    <t>RF001-TC001</t>
+  </si>
+  <si>
+    <t>RF001-TC002</t>
+  </si>
+  <si>
+    <t>RF001-TC003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permitir o cadastro no sistema utilizando email e senha	</t>
+  </si>
+  <si>
+    <t>Email do usuário =  carlos@gmail.com  Senha do usuário = carlos123</t>
+  </si>
+  <si>
+    <t>Permitir que o cadastro seja efetuado com sucesso</t>
+  </si>
+  <si>
+    <t>Não permitir o cadastro no sistema utilizando senhas diferentes</t>
+  </si>
+  <si>
+    <t>Abrir o site http://paiotnela.azurewebsites.net/, selecionar a opção/menu CADASTRO;preencher o campo de ''confirmar senha'' diferente do ''campo senha''</t>
+  </si>
+  <si>
+    <t>Senha = Carlos123 Confirme sua senha = Carlos456</t>
+  </si>
+  <si>
+    <t>Exibir a mensagem de erro "As senhas devem ser iguais";</t>
+  </si>
+  <si>
+    <t>Redirecionar o usuário para a tela de ''início'' do site após o cadastro ser efetuado com sucesso</t>
+  </si>
+  <si>
+    <t>Abrir o site http://paiotnela.azurewebsites.net/, selecionar a opção/menu CADASTRO; preencher todos os campos obrigatórios corretamente e finalizar o cadstro</t>
+  </si>
+  <si>
+    <t>Abrir o site http://paiotnela.azurewebsites.net/, selecionar a opção/menu CADASTRO;preencher todos os campos obrigatórios corretamente</t>
+  </si>
+  <si>
+    <t>Usuário é automaticamente logado após terminar o cadastro com sucesso e é redirecionado para a tela de ''Início''</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A </t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1030,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1258,6 +1276,85 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1282,13 +1379,6 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1300,74 +1390,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1497,72 +1519,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>129294</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1495425</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>947219</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagem 5" descr="Resultado de imagem para tela de cadastro">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{912CB92F-ACFA-418B-A2FE-A5D0AE3FEF1C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipV="1">
-          <a:off x="11601450" y="4872744"/>
-          <a:ext cx="1019175" cy="817925"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1888,7 +1844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C20" sqref="C20:D20"/>
     </sheetView>
   </sheetViews>
@@ -1926,13 +1882,13 @@
     </row>
     <row r="2" spans="1:20" s="22" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51"/>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="77"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="99"/>
       <c r="G2" s="55"/>
       <c r="H2" s="55"/>
       <c r="I2" s="55"/>
@@ -1942,11 +1898,11 @@
     </row>
     <row r="3" spans="1:20" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="51"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="80"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="102"/>
       <c r="G3" s="55"/>
       <c r="H3" s="55"/>
       <c r="I3" s="55"/>
@@ -1973,10 +1929,10 @@
       <c r="B5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="81" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="82"/>
+      <c r="C5" s="103" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="104"/>
       <c r="E5" s="27"/>
       <c r="F5" s="28"/>
       <c r="G5" s="27"/>
@@ -1991,8 +1947,8 @@
       <c r="B6" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="82"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="104"/>
       <c r="E6" s="27"/>
       <c r="F6" s="28"/>
       <c r="G6" s="27"/>
@@ -2007,10 +1963,10 @@
       <c r="B7" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="81">
+      <c r="C7" s="103">
         <v>1</v>
       </c>
-      <c r="D7" s="82"/>
+      <c r="D7" s="104"/>
       <c r="E7" s="27"/>
       <c r="F7" s="28"/>
       <c r="G7" s="27"/>
@@ -2025,10 +1981,10 @@
       <c r="B8" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="81">
+      <c r="C8" s="103">
         <v>6</v>
       </c>
-      <c r="D8" s="82"/>
+      <c r="D8" s="104"/>
       <c r="E8" s="27"/>
       <c r="F8" s="28"/>
       <c r="G8" s="27"/>
@@ -2041,12 +1997,12 @@
     <row r="9" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="85">
+        <v>96</v>
+      </c>
+      <c r="C9" s="105">
         <v>43614</v>
       </c>
-      <c r="D9" s="82"/>
+      <c r="D9" s="104"/>
       <c r="E9" s="27"/>
       <c r="F9" s="28"/>
       <c r="G9" s="27"/>
@@ -2072,16 +2028,16 @@
     </row>
     <row r="11" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
-      <c r="B11" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="87"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="87"/>
-      <c r="H11" s="87"/>
-      <c r="I11" s="88"/>
+      <c r="B11" s="106" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="107"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="107"/>
+      <c r="H11" s="107"/>
+      <c r="I11" s="108"/>
       <c r="J11" s="27"/>
       <c r="K11" s="27"/>
       <c r="L11" s="23"/>
@@ -2091,16 +2047,16 @@
     <row r="12" spans="1:20" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="52"/>
       <c r="B12" s="68" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="94" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="95"/>
-      <c r="E12" s="94" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="95"/>
+        <v>50</v>
+      </c>
+      <c r="C12" s="86" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="87"/>
+      <c r="E12" s="86" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="87"/>
       <c r="G12" s="68" t="s">
         <v>23</v>
       </c>
@@ -2121,24 +2077,24 @@
     <row r="13" spans="1:20" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52"/>
       <c r="B13" s="61" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="83" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="84"/>
-      <c r="E13" s="96" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="97"/>
+        <v>53</v>
+      </c>
+      <c r="C13" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="96"/>
+      <c r="E13" s="80" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="88"/>
       <c r="G13" s="62" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H13" s="73">
         <v>43617</v>
       </c>
       <c r="I13" s="62" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="J13" s="60"/>
       <c r="K13" s="60"/>
@@ -2151,24 +2107,24 @@
     <row r="14" spans="1:20" s="4" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="52"/>
       <c r="B14" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="103" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="104"/>
-      <c r="E14" s="98" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="99"/>
+        <v>54</v>
+      </c>
+      <c r="C14" s="94" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="95"/>
+      <c r="E14" s="89" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="90"/>
       <c r="G14" s="70" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H14" s="74">
         <v>43617</v>
       </c>
       <c r="I14" s="70" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="J14" s="60"/>
       <c r="K14" s="60"/>
@@ -2181,24 +2137,24 @@
     <row r="15" spans="1:20" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="52"/>
       <c r="B15" s="61" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="83" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="84"/>
-      <c r="E15" s="83" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="100"/>
+        <v>55</v>
+      </c>
+      <c r="C15" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="96"/>
+      <c r="E15" s="78" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="91"/>
       <c r="G15" s="62" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H15" s="73">
         <v>43617</v>
       </c>
       <c r="I15" s="62" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="J15" s="60"/>
       <c r="K15" s="60"/>
@@ -2211,10 +2167,10 @@
     <row r="16" spans="1:20" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="52"/>
       <c r="B16" s="61"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="91"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="79"/>
       <c r="G16" s="62"/>
       <c r="H16" s="62"/>
       <c r="I16" s="62"/>
@@ -2246,17 +2202,17 @@
     </row>
     <row r="18" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="53"/>
-      <c r="B18" s="101" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="102"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="102"/>
-      <c r="F18" s="102"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="102"/>
-      <c r="I18" s="102"/>
-      <c r="J18" s="102"/>
+      <c r="B18" s="92" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="93"/>
       <c r="K18" s="23"/>
       <c r="L18" s="23"/>
     </row>
@@ -2265,18 +2221,18 @@
       <c r="B19" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="89" t="s">
+      <c r="C19" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="90"/>
-      <c r="E19" s="89" t="s">
+      <c r="D19" s="85"/>
+      <c r="E19" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="90"/>
-      <c r="G19" s="89" t="s">
+      <c r="F19" s="85"/>
+      <c r="G19" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="90"/>
+      <c r="H19" s="85"/>
       <c r="I19" s="67" t="s">
         <v>25</v>
       </c>
@@ -2293,25 +2249,25 @@
     <row r="20" spans="1:21" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="52"/>
       <c r="B20" s="61" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="83" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="91"/>
-      <c r="E20" s="83" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" s="91"/>
-      <c r="G20" s="83" t="s">
-        <v>109</v>
-      </c>
-      <c r="H20" s="91"/>
+        <v>112</v>
+      </c>
+      <c r="C20" s="78" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="79"/>
+      <c r="E20" s="78" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="79"/>
+      <c r="G20" s="78" t="s">
+        <v>104</v>
+      </c>
+      <c r="H20" s="79"/>
       <c r="I20" s="72" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J20" s="62" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="K20" s="26"/>
       <c r="L20" s="26"/>
@@ -2323,25 +2279,25 @@
     <row r="21" spans="1:21" s="4" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="52"/>
       <c r="B21" s="61" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" s="83" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="91"/>
-      <c r="E21" s="96" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="79"/>
+      <c r="E21" s="80" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="81"/>
+      <c r="G21" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="107"/>
-      <c r="G21" s="92" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21" s="93"/>
+      <c r="H21" s="83"/>
       <c r="I21" s="71" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J21" s="62" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="K21" s="26"/>
       <c r="L21" s="26"/>
@@ -2353,25 +2309,25 @@
     <row r="22" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="52"/>
       <c r="B22" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="C22" s="83" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="79"/>
+      <c r="E22" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="81"/>
+      <c r="G22" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="91"/>
-      <c r="E22" s="96" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="107"/>
-      <c r="G22" s="92" t="s">
-        <v>74</v>
-      </c>
-      <c r="H22" s="93"/>
+      <c r="H22" s="83"/>
       <c r="I22" s="71" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J22" s="62" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="K22" s="26"/>
       <c r="L22" s="26"/>
@@ -2383,12 +2339,12 @@
     <row r="23" spans="1:21" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="52"/>
       <c r="B23" s="61"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="91"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="106"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="77"/>
       <c r="I23" s="71"/>
       <c r="J23" s="62"/>
       <c r="K23" s="26"/>
@@ -2530,16 +2486,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B11:I11"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="G21:H21"/>
@@ -2554,16 +2510,16 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E21:F21"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -2583,29 +2539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE71A8AE-B48B-47A4-89E4-FC6E9498B6A0}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3789AE18-4597-4D32-AB6F-5D09D1BF2E34}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2634,7 +2572,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2650,7 +2588,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2682,12 +2620,12 @@
         <v>36</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B10" s="38" t="s">
         <v>35</v>
@@ -2695,7 +2633,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B11" s="38" t="s">
         <v>34</v>
@@ -2713,11 +2651,11 @@
       <c r="A15" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="108" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="108"/>
-      <c r="D15" s="40"/>
+      <c r="B15" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="109"/>
+      <c r="D15" s="75"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
@@ -2747,7 +2685,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="65" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D24" s="65" t="s">
         <v>45</v>
@@ -2772,21 +2710,21 @@
       <c r="S24" s="43"/>
       <c r="T24" s="43"/>
     </row>
-    <row r="25" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A25" s="41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="D25" s="44" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="E25" s="44" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="F25" s="45"/>
       <c r="G25" s="46" t="s">
@@ -2796,129 +2734,103 @@
         <v>30</v>
       </c>
       <c r="I25" s="50" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Q25" s="43"/>
       <c r="R25" s="43"/>
       <c r="S25" s="43"/>
       <c r="T25" s="43"/>
     </row>
-    <row r="26" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A26" s="41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="D26" s="44" t="s">
-        <v>83</v>
+        <v>127</v>
       </c>
       <c r="E26" s="44" t="s">
-        <v>84</v>
+        <v>128</v>
       </c>
       <c r="F26" s="45"/>
       <c r="G26" s="46" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H26" s="46" t="s">
-        <v>115</v>
+        <v>48</v>
       </c>
       <c r="I26" s="50" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Q26" s="43"/>
       <c r="R26" s="43"/>
       <c r="S26" s="43"/>
       <c r="T26" s="43"/>
     </row>
-    <row r="27" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" s="41" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="D27" s="44" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="F27" s="45"/>
       <c r="G27" s="46" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H27" s="46" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="I27" s="50" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Q27" s="43"/>
       <c r="R27" s="43"/>
       <c r="S27" s="43"/>
       <c r="T27" s="43"/>
     </row>
-    <row r="28" spans="1:20" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="A28" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="B28" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="44" t="s">
-        <v>127</v>
-      </c>
+    <row r="28" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="41"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="44"/>
-      <c r="E28" s="44" t="s">
-        <v>125</v>
-      </c>
+      <c r="E28" s="44"/>
       <c r="F28" s="45"/>
-      <c r="G28" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="H28" s="46" t="s">
-        <v>30</v>
-      </c>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
       <c r="I28" s="50" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Q28" s="43"/>
       <c r="R28" s="43"/>
       <c r="S28" s="43"/>
       <c r="T28" s="43"/>
     </row>
-    <row r="29" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A29" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="B29" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="44" t="s">
+    <row r="29" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="50" t="s">
         <v>48</v>
-      </c>
-      <c r="E29" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="45"/>
-      <c r="G29" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="I29" s="50" t="s">
-        <v>51</v>
       </c>
       <c r="Q29" s="43"/>
       <c r="R29" s="43"/>
@@ -2996,7 +2908,408 @@
         <v>4</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>100</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="49">
+        <v>43172</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A41" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B15:C15"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{E794ACB1-865B-4804-84B8-749CA39E1601}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{E0E190C3-1DCA-4CB6-9429-937244AFB06E}"/>
+  </hyperlinks>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0" footer="9.8611111111111122E-2"/>
+  <pageSetup fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <headerFooter alignWithMargins="0">
+    <oddFooter>&amp;CSeite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:T41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" style="32" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" style="32" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" style="32" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" style="32" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="32" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" style="32" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" style="32" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" style="32" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" style="32" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="32" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" style="32" customWidth="1"/>
+    <col min="15" max="15" width="32.28515625" style="34" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" style="32" customWidth="1"/>
+    <col min="17" max="16384" width="11.7109375" style="32"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="35">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="30"/>
+      <c r="B6" s="36"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="30"/>
+      <c r="B7" s="36"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="36"/>
+      <c r="B12" s="38"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="36"/>
+      <c r="B13" s="38"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="109"/>
+      <c r="D15" s="40"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18" s="32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" s="32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="43"/>
+      <c r="S24" s="43"/>
+      <c r="T24" s="43"/>
+    </row>
+    <row r="25" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+      <c r="A25" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" s="45"/>
+      <c r="G25" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="43"/>
+      <c r="S25" s="43"/>
+      <c r="T25" s="43"/>
+    </row>
+    <row r="26" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+      <c r="A26" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="45"/>
+      <c r="G26" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="I26" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="43"/>
+    </row>
+    <row r="27" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+      <c r="A27" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" s="45"/>
+      <c r="G27" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="I27" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="43"/>
+      <c r="T27" s="43"/>
+    </row>
+    <row r="28" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="41"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="43"/>
+    </row>
+    <row r="29" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q29" s="43"/>
+      <c r="R29" s="43"/>
+      <c r="S29" s="43"/>
+      <c r="T29" s="43"/>
+    </row>
+    <row r="30" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="41"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="43"/>
+      <c r="S30" s="43"/>
+      <c r="T30" s="43"/>
+    </row>
+    <row r="31" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="41"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="43"/>
+      <c r="T31" s="43"/>
+    </row>
+    <row r="32" spans="1:20" s="42" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="41"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="43"/>
+      <c r="T32" s="43"/>
+    </row>
+    <row r="33" spans="1:20" s="42" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="41"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="Q33" s="43"/>
+      <c r="R33" s="43"/>
+      <c r="S33" s="43"/>
+      <c r="T33" s="43"/>
+    </row>
+    <row r="34" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="Q34" s="43"/>
+      <c r="R34" s="43"/>
+      <c r="S34" s="43"/>
+      <c r="T34" s="43"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A36" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
@@ -3024,7 +3337,6 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -3050,20 +3362,20 @@
     <row r="1" spans="1:6" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:6" s="17" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="64"/>
-      <c r="B2" s="109" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="111"/>
+      <c r="B2" s="110" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="112"/>
     </row>
     <row r="3" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="112"/>
-      <c r="C3" s="113"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="113"/>
-      <c r="F3" s="114"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="115"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="8"/>
@@ -3092,10 +3404,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>11</v>
@@ -3107,10 +3419,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>11</v>
@@ -3122,10 +3434,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>11</v>
@@ -3137,10 +3449,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>11</v>
@@ -3152,10 +3464,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>11</v>
@@ -3167,10 +3479,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>11</v>
@@ -3182,10 +3494,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>11</v>
@@ -3197,10 +3509,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>11</v>
@@ -3258,30 +3570,30 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="14"/>
-      <c r="C22" s="115"/>
-      <c r="D22" s="115"/>
-      <c r="E22" s="115"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="116"/>
+      <c r="E22" s="116"/>
       <c r="F22" s="15"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="116" t="s">
+      <c r="B23" s="117" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="117"/>
-      <c r="E23" s="117"/>
-      <c r="F23" s="117"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="118"/>
+      <c r="F23" s="118"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="116"/>
+      <c r="B24" s="117"/>
       <c r="C24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="117"/>
-      <c r="E24" s="117"/>
-      <c r="F24" s="117"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="118"/>
+      <c r="F24" s="118"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B27" s="12"/>
@@ -3424,13 +3736,402 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA91452-5234-4D44-A0AF-539C14598D39}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{390065AE-1EF5-437D-B6DC-1B7370DC8413}">
+  <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" style="32" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" style="32" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" style="32" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" style="32" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="32" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" style="32" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" style="32" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" style="32" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" style="32" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="32" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" style="32" customWidth="1"/>
+    <col min="15" max="15" width="32.28515625" style="34" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" style="32" customWidth="1"/>
+    <col min="17" max="16384" width="11.7109375" style="32"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="35">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="30"/>
+      <c r="B6" s="36"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="30"/>
+      <c r="B7" s="36"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="36"/>
+      <c r="B12" s="38"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="36"/>
+      <c r="B13" s="38"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="109"/>
+      <c r="D15" s="75"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18" s="32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" s="32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="43"/>
+      <c r="S24" s="43"/>
+      <c r="T24" s="43"/>
+    </row>
+    <row r="25" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A25" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="45"/>
+      <c r="G25" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="43"/>
+      <c r="S25" s="43"/>
+      <c r="T25" s="43"/>
+    </row>
+    <row r="26" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A26" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" s="45"/>
+      <c r="G26" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="43"/>
+    </row>
+    <row r="27" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A27" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="45"/>
+      <c r="G27" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="I27" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="43"/>
+      <c r="T27" s="43"/>
+    </row>
+    <row r="28" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="41"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="43"/>
+    </row>
+    <row r="29" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q29" s="43"/>
+      <c r="R29" s="43"/>
+      <c r="S29" s="43"/>
+      <c r="T29" s="43"/>
+    </row>
+    <row r="30" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="41"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="43"/>
+      <c r="S30" s="43"/>
+      <c r="T30" s="43"/>
+    </row>
+    <row r="31" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="41"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="43"/>
+      <c r="T31" s="43"/>
+    </row>
+    <row r="32" spans="1:20" s="42" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="41"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="43"/>
+      <c r="T32" s="43"/>
+    </row>
+    <row r="33" spans="1:20" s="42" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="41"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="Q33" s="43"/>
+      <c r="R33" s="43"/>
+      <c r="S33" s="43"/>
+      <c r="T33" s="43"/>
+    </row>
+    <row r="34" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="Q34" s="43"/>
+      <c r="R34" s="43"/>
+      <c r="S34" s="43"/>
+      <c r="T34" s="43"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A36" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="49">
+        <v>43172</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A41" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B15:C15"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{61ED6A7B-0C0C-4F5B-972F-7A901925C18C}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{EB341AE0-62BF-4F5D-942D-1B649F26264A}"/>
+  </hyperlinks>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0" footer="9.8611111111111122E-2"/>
+  <pageSetup fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <headerFooter alignWithMargins="0">
+    <oddFooter>&amp;CSeite &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mexi dnv pt 2
</commit_message>
<xml_diff>
--- a/documentacao/planilha-de-homo/Plano-de-UAT-homologacao.xlsx
+++ b/documentacao/planilha-de-homo/Plano-de-UAT-homologacao.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Regin\OneDrive\Documents\PI\paiotnela\documentacao\planilha-de-homo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8986EE80-9C64-4772-924D-BBA97AF6FE1F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="596" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="596" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Homologação" sheetId="5" r:id="rId1"/>
@@ -24,12 +23,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>move0011</author>
   </authors>
   <commentList>
-    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="I19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="145">
   <si>
     <t xml:space="preserve">Projeto: </t>
   </si>
@@ -290,9 +289,6 @@
     <t>Email do usuário =  EmailErrado.gmail.com</t>
   </si>
   <si>
-    <t>Exibir a mensagem de erro "Email/Login Inválido"; voltar para campo Login</t>
-  </si>
-  <si>
     <t>Email do usuário =  null/em branco</t>
   </si>
   <si>
@@ -386,9 +382,6 @@
     <t xml:space="preserve">OK </t>
   </si>
   <si>
-    <t>Exibir a mensagem de erro "Preenche este campo"; voltar para campo Login</t>
-  </si>
-  <si>
     <t>RF001</t>
   </si>
   <si>
@@ -453,12 +446,51 @@
   </si>
   <si>
     <t xml:space="preserve">N/A </t>
+  </si>
+  <si>
+    <t>Exibir os gráficos de temperatura e umdiade</t>
+  </si>
+  <si>
+    <t>Abrir o site http://paiotnela.azurewebsites.net/, selecionar a opção/menu EM ANDAMENTO; mostrar os gráficos de temperatura e umidade</t>
+  </si>
+  <si>
+    <t>Seja exibido em gráficos os valores de temperatura e umdiade</t>
+  </si>
+  <si>
+    <t>Abrir o site http://paiotnela.azurewebsites.net/, selecionar a opção/menu EM ANDAMENTO;erro ao mostrar os gráficos de temperatura e umidade</t>
+  </si>
+  <si>
+    <t>Que o gráfico não tenha nenhum valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  N/A</t>
+  </si>
+  <si>
+    <t>Não exibir os gráficos de temperatura e umdiade</t>
+  </si>
+  <si>
+    <t>Exibir apenas um dos gráficos</t>
+  </si>
+  <si>
+    <t>Abrir o site http://paiotnela.azurewebsites.net/, selecionar a opção/menu EM ANDAMENTO;erro ao mostrar um dos gráficos de temperatura e umidade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seja exibido somente um dos gráficos com valores representados </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exibir a mensagem de erro "Preenche este campo"; </t>
+  </si>
+  <si>
+    <t>Exibir a mensagem de erro "Email/Login Inválido";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   N/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
   </numFmts>
@@ -1280,6 +1312,105 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1288,109 +1419,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1424,21 +1456,21 @@
     </xf>
   </cellXfs>
   <cellStyles count="15">
-    <cellStyle name="Background" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Card" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Card B" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Card BL" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Card BR" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Card L" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Card R" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Card T" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Card TL" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Card TR" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Column Header" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Background" xfId="1"/>
+    <cellStyle name="Card" xfId="2"/>
+    <cellStyle name="Card B" xfId="3"/>
+    <cellStyle name="Card BL" xfId="4"/>
+    <cellStyle name="Card BR" xfId="5"/>
+    <cellStyle name="Card L" xfId="6"/>
+    <cellStyle name="Card R" xfId="7"/>
+    <cellStyle name="Card T" xfId="8"/>
+    <cellStyle name="Card TL" xfId="9"/>
+    <cellStyle name="Card TR" xfId="10"/>
+    <cellStyle name="Column Header" xfId="11"/>
     <cellStyle name="Hiperlink" xfId="12" builtinId="8"/>
-    <cellStyle name="Input" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Input" xfId="13"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 2" xfId="14"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1521,6 +1553,211 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>121750</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>313764</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2061882</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1142999</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11249191" y="5076264"/>
+          <a:ext cx="1940132" cy="829235"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123267</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2039473</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1097637</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11250708" y="5961529"/>
+          <a:ext cx="1916206" cy="1041608"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>56030</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2028265</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1014518</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11183471" y="4852147"/>
+          <a:ext cx="1972235" cy="924871"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>78441</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>124181</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2129117</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1277471</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11205882" y="7363181"/>
+          <a:ext cx="2050676" cy="1153290"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>246529</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>89646</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1882588</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1210236</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11373970" y="5995146"/>
+          <a:ext cx="1636059" cy="1120590"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -1597,23 +1834,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1649,23 +1869,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1841,7 +2044,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -1882,13 +2085,13 @@
     </row>
     <row r="2" spans="1:20" s="22" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51"/>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="99"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="78"/>
       <c r="G2" s="55"/>
       <c r="H2" s="55"/>
       <c r="I2" s="55"/>
@@ -1898,11 +2101,11 @@
     </row>
     <row r="3" spans="1:20" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="51"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="102"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="81"/>
       <c r="G3" s="55"/>
       <c r="H3" s="55"/>
       <c r="I3" s="55"/>
@@ -1929,10 +2132,10 @@
       <c r="B5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="104"/>
+      <c r="C5" s="82" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="83"/>
       <c r="E5" s="27"/>
       <c r="F5" s="28"/>
       <c r="G5" s="27"/>
@@ -1947,8 +2150,8 @@
       <c r="B6" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="104"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="83"/>
       <c r="E6" s="27"/>
       <c r="F6" s="28"/>
       <c r="G6" s="27"/>
@@ -1963,10 +2166,10 @@
       <c r="B7" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="103">
+      <c r="C7" s="82">
         <v>1</v>
       </c>
-      <c r="D7" s="104"/>
+      <c r="D7" s="83"/>
       <c r="E7" s="27"/>
       <c r="F7" s="28"/>
       <c r="G7" s="27"/>
@@ -1981,10 +2184,10 @@
       <c r="B8" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="103">
+      <c r="C8" s="82">
         <v>6</v>
       </c>
-      <c r="D8" s="104"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="27"/>
       <c r="F8" s="28"/>
       <c r="G8" s="27"/>
@@ -1997,12 +2200,12 @@
     <row r="9" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="59" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="105">
+        <v>95</v>
+      </c>
+      <c r="C9" s="86">
         <v>43614</v>
       </c>
-      <c r="D9" s="104"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="27"/>
       <c r="F9" s="28"/>
       <c r="G9" s="27"/>
@@ -2028,16 +2231,16 @@
     </row>
     <row r="11" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
-      <c r="B11" s="106" t="s">
+      <c r="B11" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="107"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="107"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="108"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="89"/>
       <c r="J11" s="27"/>
       <c r="K11" s="27"/>
       <c r="L11" s="23"/>
@@ -2049,14 +2252,14 @@
       <c r="B12" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="86" t="s">
+      <c r="C12" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="87"/>
-      <c r="E12" s="86" t="s">
+      <c r="D12" s="96"/>
+      <c r="E12" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="87"/>
+      <c r="F12" s="96"/>
       <c r="G12" s="68" t="s">
         <v>23</v>
       </c>
@@ -2079,22 +2282,22 @@
       <c r="B13" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="78" t="s">
+      <c r="C13" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="96"/>
-      <c r="E13" s="80" t="s">
+      <c r="D13" s="85"/>
+      <c r="E13" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="88"/>
+      <c r="F13" s="98"/>
       <c r="G13" s="62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H13" s="73">
         <v>43617</v>
       </c>
       <c r="I13" s="62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J13" s="60"/>
       <c r="K13" s="60"/>
@@ -2109,22 +2312,22 @@
       <c r="B14" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="94" t="s">
+      <c r="C14" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="95"/>
-      <c r="E14" s="89" t="s">
+      <c r="D14" s="105"/>
+      <c r="E14" s="99" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="90"/>
+      <c r="F14" s="100"/>
       <c r="G14" s="70" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H14" s="74">
         <v>43617</v>
       </c>
       <c r="I14" s="70" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J14" s="60"/>
       <c r="K14" s="60"/>
@@ -2139,22 +2342,22 @@
       <c r="B15" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="78" t="s">
+      <c r="C15" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="96"/>
-      <c r="E15" s="78" t="s">
+      <c r="D15" s="85"/>
+      <c r="E15" s="84" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="91"/>
+      <c r="F15" s="101"/>
       <c r="G15" s="62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H15" s="73">
         <v>43617</v>
       </c>
       <c r="I15" s="62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J15" s="60"/>
       <c r="K15" s="60"/>
@@ -2167,10 +2370,10 @@
     <row r="16" spans="1:20" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="52"/>
       <c r="B16" s="61"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="79"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="92"/>
       <c r="G16" s="62"/>
       <c r="H16" s="62"/>
       <c r="I16" s="62"/>
@@ -2202,17 +2405,17 @@
     </row>
     <row r="18" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="53"/>
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-      <c r="I18" s="93"/>
-      <c r="J18" s="93"/>
+      <c r="C18" s="103"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="103"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="103"/>
+      <c r="I18" s="103"/>
+      <c r="J18" s="103"/>
       <c r="K18" s="23"/>
       <c r="L18" s="23"/>
     </row>
@@ -2221,18 +2424,18 @@
       <c r="B19" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="84" t="s">
+      <c r="C19" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="85"/>
-      <c r="E19" s="84" t="s">
+      <c r="D19" s="91"/>
+      <c r="E19" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="85"/>
-      <c r="G19" s="84" t="s">
+      <c r="F19" s="91"/>
+      <c r="G19" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="85"/>
+      <c r="H19" s="91"/>
       <c r="I19" s="67" t="s">
         <v>25</v>
       </c>
@@ -2249,25 +2452,25 @@
     <row r="20" spans="1:21" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="52"/>
       <c r="B20" s="61" t="s">
-        <v>112</v>
-      </c>
-      <c r="C20" s="78" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="79"/>
-      <c r="E20" s="78" t="s">
+      <c r="D20" s="92"/>
+      <c r="E20" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="79"/>
-      <c r="G20" s="78" t="s">
+      <c r="F20" s="92"/>
+      <c r="G20" s="84" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="92"/>
+      <c r="I20" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="H20" s="79"/>
-      <c r="I20" s="72" t="s">
+      <c r="J20" s="62" t="s">
         <v>105</v>
-      </c>
-      <c r="J20" s="62" t="s">
-        <v>106</v>
       </c>
       <c r="K20" s="26"/>
       <c r="L20" s="26"/>
@@ -2279,25 +2482,25 @@
     <row r="21" spans="1:21" s="4" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="52"/>
       <c r="B21" s="61" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="78" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="79"/>
-      <c r="E21" s="80" t="s">
+      <c r="D21" s="92"/>
+      <c r="E21" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="81"/>
-      <c r="G21" s="82" t="s">
+      <c r="F21" s="108"/>
+      <c r="G21" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="83"/>
+      <c r="H21" s="94"/>
       <c r="I21" s="71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J21" s="62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K21" s="26"/>
       <c r="L21" s="26"/>
@@ -2309,25 +2512,25 @@
     <row r="22" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="52"/>
       <c r="B22" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="C22" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="79"/>
-      <c r="E22" s="80" t="s">
+      <c r="D22" s="92"/>
+      <c r="E22" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="81"/>
-      <c r="G22" s="82" t="s">
+      <c r="F22" s="108"/>
+      <c r="G22" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="83"/>
+      <c r="H22" s="94"/>
       <c r="I22" s="71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J22" s="62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K22" s="26"/>
       <c r="L22" s="26"/>
@@ -2339,12 +2542,12 @@
     <row r="23" spans="1:21" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="52"/>
       <c r="B23" s="61"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="79"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="77"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="92"/>
+      <c r="G23" s="106"/>
+      <c r="H23" s="107"/>
       <c r="I23" s="71"/>
       <c r="J23" s="62"/>
       <c r="K23" s="26"/>
@@ -2486,16 +2689,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="G21:H21"/>
@@ -2510,25 +2713,25 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B11:I11"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16">
       <formula1>"Não Iniciado, Em andamento, Concluído, Pendente"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J20:J23" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J20:J23">
       <formula1>"Não testado,Testado- NÃO OK,Testado - OK"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I20:I23" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I20:I23">
       <formula1>"Essencial, Importante, Desejável"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2539,11 +2742,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3789AE18-4597-4D32-AB6F-5D09D1BF2E34}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2588,7 +2791,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2620,7 +2823,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2685,7 +2888,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="65" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D24" s="65" t="s">
         <v>45</v>
@@ -2712,19 +2915,19 @@
     </row>
     <row r="25" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A25" s="41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B25" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="E25" s="44" t="s">
         <v>122</v>
-      </c>
-      <c r="C25" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>124</v>
       </c>
       <c r="F25" s="45"/>
       <c r="G25" s="46" t="s">
@@ -2743,21 +2946,23 @@
     </row>
     <row r="26" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A26" s="41" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B26" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="E26" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="D26" s="44" t="s">
-        <v>127</v>
-      </c>
-      <c r="E26" s="44" t="s">
-        <v>128</v>
-      </c>
-      <c r="F26" s="45"/>
+      <c r="F26" s="45" t="s">
+        <v>144</v>
+      </c>
       <c r="G26" s="46" t="s">
         <v>48</v>
       </c>
@@ -2774,26 +2979,28 @@
     </row>
     <row r="27" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="C27" s="44" t="s">
+      <c r="E27" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="D27" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="E27" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="F27" s="45"/>
+      <c r="F27" s="45" t="s">
+        <v>137</v>
+      </c>
       <c r="G27" s="46" t="s">
         <v>48</v>
       </c>
       <c r="H27" s="46" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I27" s="50" t="s">
         <v>48</v>
@@ -2908,7 +3115,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
@@ -2927,8 +3134,8 @@
     <mergeCell ref="B15:C15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{E794ACB1-865B-4804-84B8-749CA39E1601}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{E0E190C3-1DCA-4CB6-9429-937244AFB06E}"/>
+    <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0" footer="9.8611111111111122E-2"/>
@@ -2936,15 +3143,16 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:A30"/>
+    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2989,7 +3197,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3021,7 +3229,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3086,7 +3294,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="65" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D24" s="65" t="s">
         <v>45</v>
@@ -3113,16 +3321,16 @@
     </row>
     <row r="25" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A25" s="41" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B25" s="41" t="s">
         <v>72</v>
       </c>
       <c r="C25" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="44" t="s">
         <v>108</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>109</v>
       </c>
       <c r="E25" s="44" t="s">
         <v>77</v>
@@ -3144,26 +3352,26 @@
     </row>
     <row r="26" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A26" s="41" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B26" s="41" t="s">
         <v>72</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D26" s="44" t="s">
         <v>78</v>
       </c>
       <c r="E26" s="44" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
       <c r="F26" s="45"/>
       <c r="G26" s="46" t="s">
         <v>30</v>
       </c>
       <c r="H26" s="46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I26" s="50" t="s">
         <v>48</v>
@@ -3175,26 +3383,28 @@
     </row>
     <row r="27" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A27" s="41" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B27" s="41" t="s">
         <v>72</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D27" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="F27" s="45"/>
+        <v>142</v>
+      </c>
+      <c r="F27" s="45" t="s">
+        <v>137</v>
+      </c>
       <c r="G27" s="46" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H27" s="46" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
       <c r="I27" s="50" t="s">
         <v>48</v>
@@ -3309,7 +3519,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
@@ -3328,8 +3538,8 @@
     <mergeCell ref="B15:C15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0" footer="9.8611111111111122E-2"/>
@@ -3337,11 +3547,12 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3404,10 +3615,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>81</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>82</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>11</v>
@@ -3419,10 +3630,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>83</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>84</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>11</v>
@@ -3434,10 +3645,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>11</v>
@@ -3449,10 +3660,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>11</v>
@@ -3464,10 +3675,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>87</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>88</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>11</v>
@@ -3479,10 +3690,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>11</v>
@@ -3494,10 +3705,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>90</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>91</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>11</v>
@@ -3509,10 +3720,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>92</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>93</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>11</v>
@@ -3736,11 +3947,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{390065AE-1EF5-437D-B6DC-1B7370DC8413}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3785,7 +3996,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3817,7 +4028,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3882,7 +4093,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="65" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D24" s="65" t="s">
         <v>45</v>
@@ -3907,21 +4118,21 @@
       <c r="S24" s="43"/>
       <c r="T24" s="43"/>
     </row>
-    <row r="25" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A25" s="41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D25" s="44" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="E25" s="44" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="F25" s="45"/>
       <c r="G25" s="46" t="s">
@@ -3940,26 +4151,26 @@
     </row>
     <row r="26" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A26" s="41" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="D26" s="44" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="E26" s="44" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F26" s="45"/>
       <c r="G26" s="46" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="H26" s="46" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="I26" s="50" t="s">
         <v>48</v>
@@ -3971,26 +4182,26 @@
     </row>
     <row r="27" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" s="41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D27" s="44" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="F27" s="45"/>
       <c r="G27" s="46" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="H27" s="46" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="I27" s="50" t="s">
         <v>48</v>
@@ -4105,7 +4316,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
@@ -4124,8 +4335,8 @@
     <mergeCell ref="B15:C15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{61ED6A7B-0C0C-4F5B-972F-7A901925C18C}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{EB341AE0-62BF-4F5D-942D-1B649F26264A}"/>
+    <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0" footer="9.8611111111111122E-2"/>
@@ -4133,5 +4344,6 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Alterações tops na dash uheueheuheu
</commit_message>
<xml_diff>
--- a/documentacao/planilha-de-homo/Plano-de-UAT-homologacao.xlsx
+++ b/documentacao/planilha-de-homo/Plano-de-UAT-homologacao.xlsx
@@ -1,34 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Projetos\paiotnela\documentacao\planilha-de-homo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D898B1-4ED8-4379-8601-21F05E2AA5F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="596" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="596" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Homologação" sheetId="5" r:id="rId1"/>
     <sheet name="Cenário 1 - Cadastro" sheetId="9" r:id="rId2"/>
     <sheet name="Cenário 2 - Login" sheetId="6" r:id="rId3"/>
-    <sheet name="." sheetId="4" r:id="rId4"/>
-    <sheet name="Cenário 3 - Dashboard" sheetId="10" r:id="rId5"/>
+    <sheet name="Cenário 3 - Dashboard" sheetId="10" r:id="rId4"/>
+    <sheet name="." sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>move0011</author>
   </authors>
   <commentList>
-    <comment ref="I19" authorId="0" shapeId="0">
+    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -349,9 +350,6 @@
     <t>Regino</t>
   </si>
   <si>
-    <t>Não Iniciado</t>
-  </si>
-  <si>
     <t>Lucas Silva</t>
   </si>
   <si>
@@ -485,12 +483,15 @@
   </si>
   <si>
     <t xml:space="preserve">                   N/A</t>
+  </si>
+  <si>
+    <t>Concluído</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
   </numFmts>
@@ -1312,6 +1313,81 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1336,13 +1412,6 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1355,74 +1424,6 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1456,21 +1457,21 @@
     </xf>
   </cellXfs>
   <cellStyles count="15">
-    <cellStyle name="Background" xfId="1"/>
-    <cellStyle name="Card" xfId="2"/>
-    <cellStyle name="Card B" xfId="3"/>
-    <cellStyle name="Card BL" xfId="4"/>
-    <cellStyle name="Card BR" xfId="5"/>
-    <cellStyle name="Card L" xfId="6"/>
-    <cellStyle name="Card R" xfId="7"/>
-    <cellStyle name="Card T" xfId="8"/>
-    <cellStyle name="Card TL" xfId="9"/>
-    <cellStyle name="Card TR" xfId="10"/>
-    <cellStyle name="Column Header" xfId="11"/>
+    <cellStyle name="Background" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Card" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Card B" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Card BL" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Card BR" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Card L" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Card R" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Card T" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Card TL" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Card TR" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Column Header" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Hiperlink" xfId="12" builtinId="8"/>
-    <cellStyle name="Input" xfId="13"/>
+    <cellStyle name="Input" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="14"/>
+    <cellStyle name="Normal 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1570,7 +1571,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1613,7 +1620,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1651,7 +1664,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1694,7 +1713,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1732,7 +1757,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1834,6 +1865,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1869,6 +1917,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2044,11 +2109,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:D20"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2085,13 +2150,13 @@
     </row>
     <row r="2" spans="1:20" s="22" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51"/>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="78"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="99"/>
       <c r="G2" s="55"/>
       <c r="H2" s="55"/>
       <c r="I2" s="55"/>
@@ -2101,11 +2166,11 @@
     </row>
     <row r="3" spans="1:20" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="51"/>
-      <c r="B3" s="79"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="81"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="102"/>
       <c r="G3" s="55"/>
       <c r="H3" s="55"/>
       <c r="I3" s="55"/>
@@ -2132,10 +2197,10 @@
       <c r="B5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="83"/>
+      <c r="D5" s="104"/>
       <c r="E5" s="27"/>
       <c r="F5" s="28"/>
       <c r="G5" s="27"/>
@@ -2150,8 +2215,8 @@
       <c r="B6" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="83"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="104"/>
       <c r="E6" s="27"/>
       <c r="F6" s="28"/>
       <c r="G6" s="27"/>
@@ -2166,10 +2231,10 @@
       <c r="B7" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="82">
+      <c r="C7" s="103">
         <v>1</v>
       </c>
-      <c r="D7" s="83"/>
+      <c r="D7" s="104"/>
       <c r="E7" s="27"/>
       <c r="F7" s="28"/>
       <c r="G7" s="27"/>
@@ -2184,10 +2249,10 @@
       <c r="B8" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="82">
+      <c r="C8" s="103">
         <v>6</v>
       </c>
-      <c r="D8" s="83"/>
+      <c r="D8" s="104"/>
       <c r="E8" s="27"/>
       <c r="F8" s="28"/>
       <c r="G8" s="27"/>
@@ -2202,10 +2267,10 @@
       <c r="B9" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="86">
+      <c r="C9" s="105">
         <v>43614</v>
       </c>
-      <c r="D9" s="83"/>
+      <c r="D9" s="104"/>
       <c r="E9" s="27"/>
       <c r="F9" s="28"/>
       <c r="G9" s="27"/>
@@ -2231,16 +2296,16 @@
     </row>
     <row r="11" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="89"/>
+      <c r="C11" s="107"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="107"/>
+      <c r="H11" s="107"/>
+      <c r="I11" s="108"/>
       <c r="J11" s="27"/>
       <c r="K11" s="27"/>
       <c r="L11" s="23"/>
@@ -2252,14 +2317,14 @@
       <c r="B12" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="96"/>
-      <c r="E12" s="95" t="s">
+      <c r="D12" s="87"/>
+      <c r="E12" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="96"/>
+      <c r="F12" s="87"/>
       <c r="G12" s="68" t="s">
         <v>23</v>
       </c>
@@ -2282,22 +2347,22 @@
       <c r="B13" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="85"/>
-      <c r="E13" s="97" t="s">
+      <c r="D13" s="96"/>
+      <c r="E13" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="98"/>
+      <c r="F13" s="88"/>
       <c r="G13" s="62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H13" s="73">
         <v>43617</v>
       </c>
       <c r="I13" s="62" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="J13" s="60"/>
       <c r="K13" s="60"/>
@@ -2312,14 +2377,14 @@
       <c r="B14" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="104" t="s">
+      <c r="C14" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="105"/>
-      <c r="E14" s="99" t="s">
+      <c r="D14" s="95"/>
+      <c r="E14" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="100"/>
+      <c r="F14" s="90"/>
       <c r="G14" s="70" t="s">
         <v>98</v>
       </c>
@@ -2327,7 +2392,7 @@
         <v>43617</v>
       </c>
       <c r="I14" s="70" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="J14" s="60"/>
       <c r="K14" s="60"/>
@@ -2342,22 +2407,22 @@
       <c r="B15" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="84" t="s">
+      <c r="C15" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="85"/>
-      <c r="E15" s="84" t="s">
+      <c r="D15" s="96"/>
+      <c r="E15" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="101"/>
+      <c r="F15" s="91"/>
       <c r="G15" s="62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H15" s="73">
         <v>43617</v>
       </c>
       <c r="I15" s="62" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J15" s="60"/>
       <c r="K15" s="60"/>
@@ -2370,10 +2435,10 @@
     <row r="16" spans="1:20" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="52"/>
       <c r="B16" s="61"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="92"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="79"/>
       <c r="G16" s="62"/>
       <c r="H16" s="62"/>
       <c r="I16" s="62"/>
@@ -2405,17 +2470,17 @@
     </row>
     <row r="18" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="53"/>
-      <c r="B18" s="102" t="s">
+      <c r="B18" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="103"/>
-      <c r="D18" s="103"/>
-      <c r="E18" s="103"/>
-      <c r="F18" s="103"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="103"/>
-      <c r="I18" s="103"/>
-      <c r="J18" s="103"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="93"/>
       <c r="K18" s="23"/>
       <c r="L18" s="23"/>
     </row>
@@ -2424,18 +2489,18 @@
       <c r="B19" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="90" t="s">
+      <c r="C19" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="91"/>
-      <c r="E19" s="90" t="s">
+      <c r="D19" s="85"/>
+      <c r="E19" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="91"/>
-      <c r="G19" s="90" t="s">
+      <c r="F19" s="85"/>
+      <c r="G19" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="91"/>
+      <c r="H19" s="85"/>
       <c r="I19" s="67" t="s">
         <v>25</v>
       </c>
@@ -2452,25 +2517,25 @@
     <row r="20" spans="1:21" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="52"/>
       <c r="B20" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="C20" s="84" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="92"/>
-      <c r="E20" s="84" t="s">
+      <c r="D20" s="79"/>
+      <c r="E20" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="92"/>
-      <c r="G20" s="84" t="s">
+      <c r="F20" s="79"/>
+      <c r="G20" s="78" t="s">
+        <v>102</v>
+      </c>
+      <c r="H20" s="79"/>
+      <c r="I20" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="H20" s="92"/>
-      <c r="I20" s="72" t="s">
+      <c r="J20" s="62" t="s">
         <v>104</v>
-      </c>
-      <c r="J20" s="62" t="s">
-        <v>105</v>
       </c>
       <c r="K20" s="26"/>
       <c r="L20" s="26"/>
@@ -2482,25 +2547,25 @@
     <row r="21" spans="1:21" s="4" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="52"/>
       <c r="B21" s="61" t="s">
-        <v>111</v>
-      </c>
-      <c r="C21" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="92"/>
-      <c r="E21" s="97" t="s">
+      <c r="D21" s="79"/>
+      <c r="E21" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="108"/>
-      <c r="G21" s="93" t="s">
+      <c r="F21" s="81"/>
+      <c r="G21" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="94"/>
+      <c r="H21" s="83"/>
       <c r="I21" s="71" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J21" s="62" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K21" s="26"/>
       <c r="L21" s="26"/>
@@ -2512,25 +2577,25 @@
     <row r="22" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="52"/>
       <c r="B22" s="61" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="84" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="92"/>
-      <c r="E22" s="97" t="s">
+      <c r="D22" s="79"/>
+      <c r="E22" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="108"/>
-      <c r="G22" s="93" t="s">
+      <c r="F22" s="81"/>
+      <c r="G22" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="94"/>
+      <c r="H22" s="83"/>
       <c r="I22" s="71" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J22" s="62" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K22" s="26"/>
       <c r="L22" s="26"/>
@@ -2542,12 +2607,12 @@
     <row r="23" spans="1:21" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="52"/>
       <c r="B23" s="61"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="92"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="92"/>
-      <c r="G23" s="106"/>
-      <c r="H23" s="107"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="77"/>
       <c r="I23" s="71"/>
       <c r="J23" s="62"/>
       <c r="K23" s="26"/>
@@ -2689,16 +2754,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B11:I11"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="G21:H21"/>
@@ -2713,25 +2778,25 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E21:F21"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Não Iniciado, Em andamento, Concluído, Pendente"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J20:J23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J20:J23" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Não testado,Testado- NÃO OK,Testado - OK"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I20:I23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I20:I23" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Essencial, Importante, Desejável"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2742,10 +2807,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -2888,7 +2953,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D24" s="65" t="s">
         <v>45</v>
@@ -2915,19 +2980,19 @@
     </row>
     <row r="25" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A25" s="41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B25" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="C25" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="D25" s="44" t="s">
+      <c r="E25" s="44" t="s">
         <v>121</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>122</v>
       </c>
       <c r="F25" s="45"/>
       <c r="G25" s="46" t="s">
@@ -2946,22 +3011,22 @@
     </row>
     <row r="26" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A26" s="41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B26" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="D26" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="D26" s="44" t="s">
+      <c r="E26" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="E26" s="44" t="s">
-        <v>126</v>
-      </c>
       <c r="F26" s="45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G26" s="46" t="s">
         <v>48</v>
@@ -2979,28 +3044,28 @@
     </row>
     <row r="27" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" s="41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B27" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="C27" s="44" t="s">
-        <v>128</v>
-      </c>
       <c r="D27" s="44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F27" s="45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G27" s="46" t="s">
         <v>48</v>
       </c>
       <c r="H27" s="46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I27" s="50" t="s">
         <v>48</v>
@@ -3134,8 +3199,8 @@
     <mergeCell ref="B15:C15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0" footer="9.8611111111111122E-2"/>
@@ -3148,10 +3213,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -3294,7 +3359,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D24" s="65" t="s">
         <v>45</v>
@@ -3321,16 +3386,16 @@
     </row>
     <row r="25" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A25" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" s="41" t="s">
         <v>72</v>
       </c>
       <c r="C25" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="44" t="s">
         <v>107</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>108</v>
       </c>
       <c r="E25" s="44" t="s">
         <v>77</v>
@@ -3352,26 +3417,26 @@
     </row>
     <row r="26" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A26" s="41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B26" s="41" t="s">
         <v>72</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D26" s="44" t="s">
         <v>78</v>
       </c>
       <c r="E26" s="44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F26" s="45"/>
       <c r="G26" s="46" t="s">
         <v>30</v>
       </c>
       <c r="H26" s="46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I26" s="50" t="s">
         <v>48</v>
@@ -3383,22 +3448,22 @@
     </row>
     <row r="27" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A27" s="41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B27" s="41" t="s">
         <v>72</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" s="44" t="s">
         <v>79</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F27" s="45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G27" s="46" t="s">
         <v>48</v>
@@ -3538,8 +3603,8 @@
     <mergeCell ref="B15:C15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0" footer="9.8611111111111122E-2"/>
@@ -3552,405 +3617,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="1.7109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="66.28515625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="28" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="11.7109375" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:6" s="17" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64"/>
-      <c r="B2" s="110" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="112"/>
-    </row>
-    <row r="3" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="113"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="115"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="19">
-        <v>1</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="19">
-        <v>2</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="21"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="19">
-        <v>3</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="19">
-        <v>4</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="21"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="19">
-        <v>5</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="21"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="19">
-        <v>6</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="21"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="19">
-        <v>7</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="19">
-        <v>8</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="21"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="14"/>
-      <c r="C22" s="116"/>
-      <c r="D22" s="116"/>
-      <c r="E22" s="116"/>
-      <c r="F22" s="15"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="117" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="118"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="118"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="117"/>
-      <c r="C24" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="118"/>
-      <c r="E24" s="118"/>
-      <c r="F24" s="118"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="13"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="13"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="13"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="13"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="13"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="13"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="13"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="13"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="13"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="13"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="13"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="13"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="13"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="13"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="13"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="13"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="13"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="13"/>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="13"/>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="13"/>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="13"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -4093,7 +3763,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D24" s="65" t="s">
         <v>45</v>
@@ -4120,19 +3790,19 @@
     </row>
     <row r="25" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A25" s="41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B25" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="D25" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25" s="44" t="s">
         <v>133</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>134</v>
       </c>
       <c r="F25" s="45"/>
       <c r="G25" s="46" t="s">
@@ -4151,19 +3821,19 @@
     </row>
     <row r="26" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A26" s="41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C26" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" s="44" t="s">
         <v>135</v>
-      </c>
-      <c r="D26" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="E26" s="44" t="s">
-        <v>136</v>
       </c>
       <c r="F26" s="45"/>
       <c r="G26" s="46" t="s">
@@ -4182,26 +3852,26 @@
     </row>
     <row r="27" spans="1:20" s="42" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" s="41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B27" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="C27" s="44" t="s">
+      <c r="D27" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="E27" s="44" t="s">
         <v>140</v>
-      </c>
-      <c r="D27" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="E27" s="44" t="s">
-        <v>141</v>
       </c>
       <c r="F27" s="45"/>
       <c r="G27" s="46" t="s">
         <v>30</v>
       </c>
       <c r="H27" s="46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I27" s="50" t="s">
         <v>48</v>
@@ -4335,8 +4005,8 @@
     <mergeCell ref="B15:C15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0" footer="9.8611111111111122E-2"/>
@@ -4346,4 +4016,399 @@
   </headerFooter>
   <drawing r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="66.28515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="28" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="11.7109375" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:6" s="17" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="64"/>
+      <c r="B2" s="110" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="112"/>
+    </row>
+    <row r="3" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="113"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="115"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="19">
+        <v>1</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="19">
+        <v>2</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="19">
+        <v>3</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="19">
+        <v>4</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="19">
+        <v>5</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="21"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="19">
+        <v>6</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="19">
+        <v>7</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="19">
+        <v>8</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="14"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="116"/>
+      <c r="E22" s="116"/>
+      <c r="F22" s="15"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="117" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="118"/>
+      <c r="E23" s="118"/>
+      <c r="F23" s="118"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="117"/>
+      <c r="C24" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="118"/>
+      <c r="E24" s="118"/>
+      <c r="F24" s="118"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="13"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="13"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="13"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="13"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="13"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="13"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="13"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="13"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="13"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="13"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="13"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="13"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="13"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="13"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="13"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="13"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="13"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="13"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>